<commit_message>
new numbers add in airtel
</commit_message>
<xml_diff>
--- a/SIM Card Details/Airtel/ACTIVATION_DOWNLOAD_TEMPLATE2021-06-26T11_51_17+05_30.xlsx
+++ b/SIM Card Details/Airtel/ACTIVATION_DOWNLOAD_TEMPLATE2021-06-26T11_51_17+05_30.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>MOBILE_NUMBER</t>
   </si>
@@ -64,100 +64,97 @@
     <t>M2ML 2G 500MB 200 SMS - INR70 PM AR</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>ACTIVATE_SIM</t>
   </si>
   <si>
-    <t>5754000558762</t>
-  </si>
-  <si>
-    <t>8991000905770767822</t>
-  </si>
-  <si>
-    <t>404490624645598</t>
-  </si>
-  <si>
-    <t>5754000558758</t>
-  </si>
-  <si>
-    <t>8991000905770767780</t>
-  </si>
-  <si>
-    <t>404490624647458</t>
-  </si>
-  <si>
-    <t>5754000558756</t>
-  </si>
-  <si>
-    <t>8991000905770767764</t>
-  </si>
-  <si>
-    <t>404490624647457</t>
-  </si>
-  <si>
-    <t>5754000558764</t>
-  </si>
-  <si>
-    <t>8991000905770767848</t>
-  </si>
-  <si>
-    <t>404490624645614</t>
-  </si>
-  <si>
-    <t>5754000558759</t>
-  </si>
-  <si>
-    <t>8991000905770767798</t>
-  </si>
-  <si>
-    <t>404490624645627</t>
-  </si>
-  <si>
-    <t>5754000558760</t>
-  </si>
-  <si>
-    <t>8991000905770767806</t>
-  </si>
-  <si>
-    <t>404490624645603</t>
-  </si>
-  <si>
-    <t>5754000558757</t>
-  </si>
-  <si>
-    <t>8991000905770767772</t>
-  </si>
-  <si>
-    <t>404490624645631</t>
-  </si>
-  <si>
-    <t>5754000558763</t>
-  </si>
-  <si>
-    <t>8991000905770767830</t>
-  </si>
-  <si>
-    <t>404490624645606</t>
-  </si>
-  <si>
-    <t>5754000558761</t>
-  </si>
-  <si>
-    <t>8991000905770767814</t>
-  </si>
-  <si>
-    <t>404490624647460</t>
-  </si>
-  <si>
-    <t>5754000558755</t>
-  </si>
-  <si>
-    <t>8991000905770767756</t>
-  </si>
-  <si>
-    <t>404490624645618</t>
+    <t>5754000558770</t>
+  </si>
+  <si>
+    <t>5754000558769</t>
+  </si>
+  <si>
+    <t>5754000558773</t>
+  </si>
+  <si>
+    <t>5754000558767</t>
+  </si>
+  <si>
+    <t>5754000558765</t>
+  </si>
+  <si>
+    <t>5754000558774</t>
+  </si>
+  <si>
+    <t>5754000558771</t>
+  </si>
+  <si>
+    <t>5754000558772</t>
+  </si>
+  <si>
+    <t>5754000558768</t>
+  </si>
+  <si>
+    <t>5754000558766</t>
+  </si>
+  <si>
+    <t>8991000905770767905</t>
+  </si>
+  <si>
+    <t>404490624645621</t>
+  </si>
+  <si>
+    <t>8991000905770767897</t>
+  </si>
+  <si>
+    <t>404490624645624</t>
+  </si>
+  <si>
+    <t>8991000905770767939</t>
+  </si>
+  <si>
+    <t>404490624645613</t>
+  </si>
+  <si>
+    <t>8991000905770767871</t>
+  </si>
+  <si>
+    <t>404490624645609</t>
+  </si>
+  <si>
+    <t>8991000905770767855</t>
+  </si>
+  <si>
+    <t>404490624647454</t>
+  </si>
+  <si>
+    <t>8991000905770767947</t>
+  </si>
+  <si>
+    <t>404490624645597</t>
+  </si>
+  <si>
+    <t>8991000905770767913</t>
+  </si>
+  <si>
+    <t>404490624645610</t>
+  </si>
+  <si>
+    <t>8991000905770767921</t>
+  </si>
+  <si>
+    <t>404490624645579</t>
+  </si>
+  <si>
+    <t>8991000905770767889</t>
+  </si>
+  <si>
+    <t>404490624645623</t>
+  </si>
+  <si>
+    <t>8991000905770767863</t>
+  </si>
+  <si>
+    <t>404490624645628</t>
   </si>
 </sst>
 </file>
@@ -531,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,13 +581,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -602,25 +599,21 @@
         <v>12</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -632,25 +625,21 @@
         <v>12</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -662,25 +651,21 @@
         <v>12</v>
       </c>
       <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -692,25 +677,21 @@
         <v>12</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -722,25 +703,21 @@
         <v>12</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>10</v>
@@ -752,25 +729,21 @@
         <v>12</v>
       </c>
       <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -782,25 +755,21 @@
         <v>12</v>
       </c>
       <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>
@@ -812,19 +781,15 @@
         <v>12</v>
       </c>
       <c r="G9" s="3"/>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>40</v>
@@ -842,25 +807,21 @@
         <v>12</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>10</v>
@@ -875,7 +836,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -944,122 +905,12 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="J2:J31">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J21">
       <formula1>"ACTIVATE_SIM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F31">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F21">
       <formula1>"M2ML 2G 500MB 200 SMS - INR70 PM AR"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
new numbers added in airtel
</commit_message>
<xml_diff>
--- a/SIM Card Details/Airtel/ACTIVATION_DOWNLOAD_TEMPLATE2021-06-26T11_51_17+05_30.xlsx
+++ b/SIM Card Details/Airtel/ACTIVATION_DOWNLOAD_TEMPLATE2021-06-26T11_51_17+05_30.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>MOBILE_NUMBER</t>
   </si>
@@ -67,94 +67,49 @@
     <t>ACTIVATE_SIM</t>
   </si>
   <si>
-    <t>5754000558770</t>
-  </si>
-  <si>
-    <t>5754000558769</t>
-  </si>
-  <si>
-    <t>5754000558773</t>
-  </si>
-  <si>
-    <t>5754000558767</t>
-  </si>
-  <si>
-    <t>5754000558765</t>
-  </si>
-  <si>
-    <t>5754000558774</t>
-  </si>
-  <si>
-    <t>5754000558771</t>
-  </si>
-  <si>
-    <t>5754000558772</t>
-  </si>
-  <si>
-    <t>5754000558768</t>
-  </si>
-  <si>
-    <t>5754000558766</t>
-  </si>
-  <si>
-    <t>8991000905770767905</t>
-  </si>
-  <si>
-    <t>404490624645621</t>
-  </si>
-  <si>
-    <t>8991000905770767897</t>
-  </si>
-  <si>
-    <t>404490624645624</t>
-  </si>
-  <si>
-    <t>8991000905770767939</t>
-  </si>
-  <si>
-    <t>404490624645613</t>
-  </si>
-  <si>
-    <t>8991000905770767871</t>
-  </si>
-  <si>
-    <t>404490624645609</t>
-  </si>
-  <si>
-    <t>8991000905770767855</t>
-  </si>
-  <si>
-    <t>404490624647454</t>
-  </si>
-  <si>
-    <t>8991000905770767947</t>
-  </si>
-  <si>
-    <t>404490624645597</t>
-  </si>
-  <si>
-    <t>8991000905770767913</t>
-  </si>
-  <si>
-    <t>404490624645610</t>
-  </si>
-  <si>
-    <t>8991000905770767921</t>
-  </si>
-  <si>
-    <t>404490624645579</t>
-  </si>
-  <si>
-    <t>8991000905770767889</t>
-  </si>
-  <si>
-    <t>404490624645623</t>
-  </si>
-  <si>
-    <t>8991000905770767863</t>
-  </si>
-  <si>
-    <t>404490624645628</t>
+    <t>5754000558778</t>
+  </si>
+  <si>
+    <t>8991000905770767988</t>
+  </si>
+  <si>
+    <t>404490624645622</t>
+  </si>
+  <si>
+    <t>5754000558777</t>
+  </si>
+  <si>
+    <t>8991000905770767970</t>
+  </si>
+  <si>
+    <t>404490624645600</t>
+  </si>
+  <si>
+    <t>5754000558776</t>
+  </si>
+  <si>
+    <t>8991000905770767962</t>
+  </si>
+  <si>
+    <t>404490624647450</t>
+  </si>
+  <si>
+    <t>5754000558775</t>
+  </si>
+  <si>
+    <t>8991000905770767954</t>
+  </si>
+  <si>
+    <t>404490624647451</t>
+  </si>
+  <si>
+    <t>5754000558779</t>
+  </si>
+  <si>
+    <t>8991000905770767996</t>
+  </si>
+  <si>
+    <t>404490624645605</t>
   </si>
 </sst>
 </file>
@@ -528,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,10 +539,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>10</v>
@@ -607,13 +562,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>10</v>
@@ -633,13 +588,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -659,13 +614,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>10</v>
@@ -685,13 +640,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
@@ -710,134 +665,63 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>12</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -894,23 +778,12 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="J2:J21">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J20">
       <formula1>"ACTIVATE_SIM"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F21">
+    <dataValidation type="list" allowBlank="1" sqref="F2:F20">
       <formula1>"M2ML 2G 500MB 200 SMS - INR70 PM AR"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>